<commit_message>
Tweaked ignition, fixed detonation
</commit_message>
<xml_diff>
--- a/tmpy_aicb.xlsx
+++ b/tmpy_aicb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upm365-my.sharepoint.com/personal/mario_deltoro_armas_alumnos_upm_es/Documents/4_GIA/cuatri_1/MAA/OTTOcompleto_V24_MAA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{36AA820A-A262-8647-9E2B-9358A6BD94F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BA01C24-3043-214F-B990-13BB449CF119}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{36AA820A-A262-8647-9E2B-9358A6BD94F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6802510A-50DE-4640-A2F7-CDEA4702E66C}"/>
   <bookViews>
     <workbookView xWindow="15180" yWindow="920" windowWidth="14900" windowHeight="18560" xr2:uid="{AD7E9AC7-CCC2-744C-95BA-C9EF2A216389}"/>
   </bookViews>
@@ -406,162 +406,162 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B1" sqref="B1:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1">
         <f>A1*2-20</f>
-        <v>-14</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B17" si="0">A2*2-20</f>
-        <v>-4</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>10.4</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>0.80000000000000071</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>13.5</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>14.5</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>15.5</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>16.600000000000001</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>13.200000000000003</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>17.5</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>17.899999999999999</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>15.799999999999997</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>18.5</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>18.899999999999999</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>17.799999999999997</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>19.3</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>18.600000000000001</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>19.600000000000001</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>19.200000000000003</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>20.2</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>20.399999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>20.5</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fine tuning of AICB parameter to prevent detonation
</commit_message>
<xml_diff>
--- a/tmpy_aicb.xlsx
+++ b/tmpy_aicb.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upm365-my.sharepoint.com/personal/mario_deltoro_armas_alumnos_upm_es/Documents/4_GIA/cuatri_1/MAA/OTTOcompleto_V24_MAA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{36AA820A-A262-8647-9E2B-9358A6BD94F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6802510A-50DE-4640-A2F7-CDEA4702E66C}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="8_{36AA820A-A262-8647-9E2B-9358A6BD94F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEEED0A3-0A27-D045-807C-5C879AF61F9B}"/>
   <bookViews>
     <workbookView xWindow="15180" yWindow="920" windowWidth="14900" windowHeight="18560" xr2:uid="{AD7E9AC7-CCC2-744C-95BA-C9EF2A216389}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,9 +66,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AC0D58-9F01-B649-A140-9A41C9184D57}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B17"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -422,146 +421,1441 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B17" si="0">A2*2-20</f>
-        <v>-6</v>
+        <f t="shared" ref="B2:B104" si="0">A2*2-20</f>
+        <v>-16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>11</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>12</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>12</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>12</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>12</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>12</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>12</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>13</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>13</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>13</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>13</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>13</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>13</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>13</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>13</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>13</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>13</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>13</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>14</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>14</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>14</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>14</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>14</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>14</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>14</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>14</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>14</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>14</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>14</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>14</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>15</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>15</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>15</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>15</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>15</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>15</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>15</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>15</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>15</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>15</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>15</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>15</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>15</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>15</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>15</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>16</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>16</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>16</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>16</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>16</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>16</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>16</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>16</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>16</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>16</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>16</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>61</v>
+      </c>
+      <c r="B95">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>16</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>16</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>16</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>16</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>16</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>17</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>17</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>17</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>17</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>17</v>
+      </c>
+      <c r="B105">
+        <f t="shared" ref="B105:B161" si="1">A105*2-20</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>17</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>17</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>17</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>17</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>17</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>17</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>17</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>17</v>
+      </c>
+      <c r="B113">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>17</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>17</v>
+      </c>
+      <c r="B115">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>17</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>17</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>17</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>17</v>
+      </c>
+      <c r="B119">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>17</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>17</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>17</v>
+      </c>
+      <c r="B122">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>18</v>
+      </c>
+      <c r="B123">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>18</v>
+      </c>
+      <c r="B124">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>18</v>
+      </c>
+      <c r="B125">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>18</v>
+      </c>
+      <c r="B126">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>18</v>
+      </c>
+      <c r="B127">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>18</v>
+      </c>
+      <c r="B128">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>18</v>
+      </c>
+      <c r="B129">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>18</v>
+      </c>
+      <c r="B130">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>18</v>
+      </c>
+      <c r="B131">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>18</v>
+      </c>
+      <c r="B132">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>18</v>
+      </c>
+      <c r="B133">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>18</v>
+      </c>
+      <c r="B134">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>18</v>
+      </c>
+      <c r="B135">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>18</v>
+      </c>
+      <c r="B136">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>18</v>
+      </c>
+      <c r="B137">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>18</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>18</v>
+      </c>
+      <c r="B139">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>18</v>
+      </c>
+      <c r="B140">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>18</v>
+      </c>
+      <c r="B141">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>18</v>
+      </c>
+      <c r="B142">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>18</v>
+      </c>
+      <c r="B143">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>18</v>
+      </c>
+      <c r="B144">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>18</v>
+      </c>
+      <c r="B145">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146">
         <v>19</v>
       </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>20</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>20</v>
+      <c r="B146">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>19</v>
+      </c>
+      <c r="B147">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>19</v>
+      </c>
+      <c r="B148">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>19</v>
+      </c>
+      <c r="B149">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>19</v>
+      </c>
+      <c r="B150">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>19</v>
+      </c>
+      <c r="B151">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>19</v>
+      </c>
+      <c r="B152">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>19</v>
+      </c>
+      <c r="B153">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>19</v>
+      </c>
+      <c r="B154">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>19</v>
+      </c>
+      <c r="B155">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>19</v>
+      </c>
+      <c r="B156">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>19</v>
+      </c>
+      <c r="B157">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>19</v>
+      </c>
+      <c r="B158">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>19</v>
+      </c>
+      <c r="B159">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>19</v>
+      </c>
+      <c r="B160">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>19</v>
+      </c>
+      <c r="B161">
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added precise labels to plots
</commit_message>
<xml_diff>
--- a/tmpy_aicb.xlsx
+++ b/tmpy_aicb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upm365-my.sharepoint.com/personal/mario_deltoro_armas_alumnos_upm_es/Documents/4_GIA/cuatri_1/MAA/OTTOcompleto_V24_MAA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="8_{36AA820A-A262-8647-9E2B-9358A6BD94F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEEED0A3-0A27-D045-807C-5C879AF61F9B}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="8_{36AA820A-A262-8647-9E2B-9358A6BD94F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F4483A2-C136-434D-8331-D31FDF59BB5C}"/>
   <bookViews>
     <workbookView xWindow="15180" yWindow="920" windowWidth="14900" windowHeight="18560" xr2:uid="{AD7E9AC7-CCC2-744C-95BA-C9EF2A216389}"/>
   </bookViews>
@@ -402,15 +402,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AC0D58-9F01-B649-A140-9A41C9184D57}">
-  <dimension ref="A1:B161"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>2</v>
       </c>
@@ -418,8 +418,11 @@
         <f>A1*2-20</f>
         <v>-16</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -427,8 +430,11 @@
         <f t="shared" ref="B2:B104" si="0">A2*2-20</f>
         <v>-16</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -436,8 +442,11 @@
         <f t="shared" si="0"/>
         <v>-14</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -445,8 +454,11 @@
         <f t="shared" si="0"/>
         <v>-12</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -454,8 +466,11 @@
         <f t="shared" si="0"/>
         <v>-12</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -463,8 +478,11 @@
         <f t="shared" si="0"/>
         <v>-12</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -472,8 +490,11 @@
         <f t="shared" si="0"/>
         <v>-10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -481,8 +502,11 @@
         <f t="shared" si="0"/>
         <v>-10</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -490,8 +514,11 @@
         <f t="shared" si="0"/>
         <v>-8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -499,8 +526,11 @@
         <f t="shared" si="0"/>
         <v>-8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>6</v>
       </c>
@@ -508,8 +538,11 @@
         <f t="shared" si="0"/>
         <v>-8</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>7</v>
       </c>
@@ -517,8 +550,11 @@
         <f t="shared" si="0"/>
         <v>-6</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7</v>
       </c>
@@ -526,8 +562,11 @@
         <f t="shared" si="0"/>
         <v>-6</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7</v>
       </c>
@@ -535,8 +574,11 @@
         <f t="shared" si="0"/>
         <v>-6</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7</v>
       </c>
@@ -544,8 +586,11 @@
         <f t="shared" si="0"/>
         <v>-6</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>
@@ -553,8 +598,11 @@
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
@@ -562,8 +610,11 @@
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>8</v>
       </c>
@@ -571,8 +622,11 @@
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8</v>
       </c>
@@ -580,8 +634,11 @@
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9</v>
       </c>
@@ -589,8 +646,11 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>9</v>
       </c>
@@ -598,8 +658,11 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9</v>
       </c>
@@ -607,8 +670,11 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>9</v>
       </c>
@@ -616,8 +682,11 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>10</v>
       </c>
@@ -625,8 +694,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>10</v>
       </c>
@@ -634,8 +706,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>10</v>
       </c>
@@ -643,8 +718,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>10</v>
       </c>
@@ -652,8 +730,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -661,8 +742,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>10</v>
       </c>
@@ -670,8 +754,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>11</v>
       </c>
@@ -679,8 +766,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>3450</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>11</v>
       </c>
@@ -688,8 +778,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>11</v>
       </c>
@@ -697,8 +790,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>3550</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>11</v>
       </c>
@@ -706,8 +802,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>11</v>
       </c>
@@ -715,8 +814,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>11</v>
       </c>
@@ -724,8 +826,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>11</v>
       </c>
@@ -733,8 +838,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>12</v>
       </c>
@@ -742,8 +850,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>12</v>
       </c>
@@ -751,8 +862,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>3850</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>12</v>
       </c>
@@ -760,8 +874,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>12</v>
       </c>
@@ -769,8 +886,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>12</v>
       </c>
@@ -778,8 +898,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>12</v>
       </c>
@@ -787,8 +910,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>4050</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>12</v>
       </c>
@@ -796,8 +922,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>12</v>
       </c>
@@ -805,8 +934,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>4150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>12</v>
       </c>
@@ -814,8 +946,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>13</v>
       </c>
@@ -823,8 +958,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <v>4250</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>13</v>
       </c>
@@ -832,8 +970,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>13</v>
       </c>
@@ -841,8 +982,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>13</v>
       </c>
@@ -850,8 +994,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>13</v>
       </c>
@@ -859,8 +1006,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>4450</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>13</v>
       </c>
@@ -868,8 +1018,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>13</v>
       </c>
@@ -877,8 +1030,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <v>4550</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>13</v>
       </c>
@@ -886,8 +1042,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>13</v>
       </c>
@@ -895,8 +1054,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>13</v>
       </c>
@@ -904,8 +1066,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>13</v>
       </c>
@@ -913,8 +1078,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>4750</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>14</v>
       </c>
@@ -922,8 +1090,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>14</v>
       </c>
@@ -931,8 +1102,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <v>4850</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>14</v>
       </c>
@@ -940,8 +1114,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>14</v>
       </c>
@@ -949,8 +1126,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <v>4950</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>14</v>
       </c>
@@ -958,8 +1138,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>14</v>
       </c>
@@ -967,8 +1150,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <v>5050</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>14</v>
       </c>
@@ -976,8 +1162,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>14</v>
       </c>
@@ -985,8 +1174,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <v>5150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>14</v>
       </c>
@@ -994,8 +1186,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D65">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>14</v>
       </c>
@@ -1003,8 +1198,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>14</v>
       </c>
@@ -1012,8 +1210,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D67">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>14</v>
       </c>
@@ -1021,8 +1222,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D68">
+        <v>5350</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>15</v>
       </c>
@@ -1030,8 +1234,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D69">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>15</v>
       </c>
@@ -1039,8 +1246,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D70">
+        <v>5450</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>15</v>
       </c>
@@ -1048,8 +1258,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D71">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>15</v>
       </c>
@@ -1057,8 +1270,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D72">
+        <v>5550</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>15</v>
       </c>
@@ -1066,8 +1282,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D73">
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>15</v>
       </c>
@@ -1075,8 +1294,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <v>5650</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>15</v>
       </c>
@@ -1084,8 +1306,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>15</v>
       </c>
@@ -1093,8 +1318,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D76">
+        <v>5750</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>15</v>
       </c>
@@ -1102,8 +1330,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>15</v>
       </c>
@@ -1111,8 +1342,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D78">
+        <v>5850</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>15</v>
       </c>
@@ -1120,8 +1354,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>15</v>
       </c>
@@ -1129,8 +1366,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D80">
+        <v>5950</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>15</v>
       </c>
@@ -1138,8 +1378,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>15</v>
       </c>
@@ -1147,8 +1390,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D82">
+        <v>6050</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>15</v>
       </c>
@@ -1156,8 +1402,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D83">
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>16</v>
       </c>
@@ -1165,8 +1414,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D84">
+        <v>6150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>16</v>
       </c>
@@ -1174,8 +1426,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>16</v>
       </c>
@@ -1183,8 +1438,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D86">
+        <v>6250</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>16</v>
       </c>
@@ -1192,8 +1450,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D87">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>16</v>
       </c>
@@ -1201,8 +1462,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D88">
+        <v>6350</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>16</v>
       </c>
@@ -1210,8 +1474,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D89">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>16</v>
       </c>
@@ -1219,8 +1486,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D90">
+        <v>6450</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>16</v>
       </c>
@@ -1228,8 +1498,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D91">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>16</v>
       </c>
@@ -1237,8 +1510,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D92">
+        <v>6550</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>16</v>
       </c>
@@ -1246,8 +1522,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D93">
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>16</v>
       </c>
@@ -1255,16 +1534,22 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D94">
+        <v>6650</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>61</v>
       </c>
       <c r="B95">
         <v>12</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D95">
+        <v>6700</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>16</v>
       </c>
@@ -1272,8 +1557,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D96">
+        <v>6750</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>16</v>
       </c>
@@ -1281,8 +1569,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D97">
+        <v>6800</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>16</v>
       </c>
@@ -1290,8 +1581,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D98">
+        <v>6850</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>16</v>
       </c>
@@ -1299,8 +1593,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D99">
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>16</v>
       </c>
@@ -1308,8 +1605,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D100">
+        <v>6950</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>17</v>
       </c>
@@ -1317,8 +1617,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D101">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>17</v>
       </c>
@@ -1326,8 +1629,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D102">
+        <v>7050</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>17</v>
       </c>
@@ -1335,8 +1641,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D103">
+        <v>7100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>17</v>
       </c>
@@ -1344,8 +1653,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D104">
+        <v>7150</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>17</v>
       </c>
@@ -1353,8 +1665,11 @@
         <f t="shared" ref="B105:B161" si="1">A105*2-20</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D105">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>17</v>
       </c>
@@ -1362,8 +1677,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D106">
+        <v>7250</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>17</v>
       </c>
@@ -1371,8 +1689,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D107">
+        <v>7300</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>17</v>
       </c>
@@ -1380,8 +1701,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D108">
+        <v>7350</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>17</v>
       </c>
@@ -1389,8 +1713,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D109">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>17</v>
       </c>
@@ -1398,8 +1725,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D110">
+        <v>7450</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>17</v>
       </c>
@@ -1407,8 +1737,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D111">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>17</v>
       </c>
@@ -1416,8 +1749,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D112">
+        <v>7550</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>17</v>
       </c>
@@ -1425,8 +1761,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D113">
+        <v>7600</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>17</v>
       </c>
@@ -1434,8 +1773,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D114">
+        <v>7650</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>17</v>
       </c>
@@ -1443,8 +1785,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D115">
+        <v>7700</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>17</v>
       </c>
@@ -1452,8 +1797,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D116">
+        <v>7750</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>17</v>
       </c>
@@ -1461,8 +1809,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D117">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>17</v>
       </c>
@@ -1470,8 +1821,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D118">
+        <v>7850</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>17</v>
       </c>
@@ -1479,8 +1833,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D119">
+        <v>7900</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>17</v>
       </c>
@@ -1488,8 +1845,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D120">
+        <v>7950</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>17</v>
       </c>
@@ -1497,8 +1857,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D121">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>17</v>
       </c>
@@ -1506,8 +1869,11 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D122">
+        <v>8050</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>18</v>
       </c>
@@ -1515,8 +1881,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D123">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>18</v>
       </c>
@@ -1524,8 +1893,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D124">
+        <v>8150</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>18</v>
       </c>
@@ -1533,8 +1905,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D125">
+        <v>8200</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>18</v>
       </c>
@@ -1542,8 +1917,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D126">
+        <v>8250</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>18</v>
       </c>
@@ -1551,8 +1929,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D127">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>18</v>
       </c>
@@ -1560,8 +1941,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D128">
+        <v>8350</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>18</v>
       </c>
@@ -1569,8 +1953,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D129">
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>18</v>
       </c>
@@ -1578,8 +1965,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D130">
+        <v>8450</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>18</v>
       </c>
@@ -1587,8 +1977,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D131">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>18</v>
       </c>
@@ -1596,8 +1989,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D132">
+        <v>8550</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>18</v>
       </c>
@@ -1605,8 +2001,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D133">
+        <v>8600</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>18</v>
       </c>
@@ -1614,8 +2013,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D134">
+        <v>8650</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>18</v>
       </c>
@@ -1623,8 +2025,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D135">
+        <v>8700</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>18</v>
       </c>
@@ -1632,8 +2037,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D136">
+        <v>8750</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>18</v>
       </c>
@@ -1641,8 +2049,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D137">
+        <v>8800</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>18</v>
       </c>
@@ -1650,8 +2061,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D138">
+        <v>8850</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>18</v>
       </c>
@@ -1659,8 +2073,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D139">
+        <v>8900</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>18</v>
       </c>
@@ -1668,8 +2085,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D140">
+        <v>8950</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>18</v>
       </c>
@@ -1677,8 +2097,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D141">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>18</v>
       </c>
@@ -1686,8 +2109,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D142">
+        <v>9050</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>18</v>
       </c>
@@ -1695,8 +2121,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D143">
+        <v>9100</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>18</v>
       </c>
@@ -1704,8 +2133,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D144">
+        <v>9150</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>18</v>
       </c>
@@ -1713,8 +2145,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D145">
+        <v>9200</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>19</v>
       </c>
@@ -1722,8 +2157,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D146">
+        <v>9250</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>19</v>
       </c>
@@ -1731,8 +2169,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D147">
+        <v>9300</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>19</v>
       </c>
@@ -1740,8 +2181,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D148">
+        <v>9350</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>19</v>
       </c>
@@ -1749,8 +2193,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D149">
+        <v>9400</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>19</v>
       </c>
@@ -1758,8 +2205,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D150">
+        <v>9450</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>19</v>
       </c>
@@ -1767,8 +2217,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D151">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>19</v>
       </c>
@@ -1776,8 +2229,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D152">
+        <v>9550</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>19</v>
       </c>
@@ -1785,8 +2241,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D153">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>19</v>
       </c>
@@ -1794,8 +2253,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D154">
+        <v>9650</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>19</v>
       </c>
@@ -1803,8 +2265,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D155">
+        <v>9700</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>19</v>
       </c>
@@ -1812,8 +2277,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D156">
+        <v>9750</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>19</v>
       </c>
@@ -1821,8 +2289,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D157">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>19</v>
       </c>
@@ -1830,8 +2301,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D158">
+        <v>9850</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>19</v>
       </c>
@@ -1839,8 +2313,11 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D159">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>19</v>
       </c>
@@ -1848,14 +2325,20 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D160">
+        <v>9950</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>19</v>
       </c>
       <c r="B161">
         <f t="shared" si="1"/>
         <v>18</v>
+      </c>
+      <c r="D161">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>